<commit_message>
refactor: :card_file_box: Refactor DataBase
</commit_message>
<xml_diff>
--- a/src/DataBase/db_istituciones.xlsx
+++ b/src/DataBase/db_istituciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SistemaSeleccionDePracticasISUS\src\DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\practicasisus\src\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F60EBA8B-CEC8-4F6C-92FF-3D8CE3D015DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473CE513-2E6F-4992-84A9-48BFFAFAEC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41072567-9FE2-431C-85BD-C400A3ED8B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{41072567-9FE2-431C-85BD-C400A3ED8B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -276,7 +276,7 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -607,11 +607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B8AC53-B0CE-4F6C-8DB1-4409F3645CAF}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
@@ -649,7 +647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -705,7 +703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -713,7 +711,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -721,7 +719,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -769,7 +767,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -785,7 +783,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -793,7 +791,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -809,7 +807,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
docs: :card_file_box: Update DataBase Instituciones
</commit_message>
<xml_diff>
--- a/src/DataBase/db_istituciones.xlsx
+++ b/src/DataBase/db_istituciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\practicasisus\src\DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SistemaSeleccionDePracticasISUS\src\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473CE513-2E6F-4992-84A9-48BFFAFAEC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9CFC4F-422C-41BC-86CB-8F5558977CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{41072567-9FE2-431C-85BD-C400A3ED8B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41072567-9FE2-431C-85BD-C400A3ED8B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>EMPRESACENTRO INFANTIL/UNIDAD EDUCATIVA</t>
   </si>
@@ -193,13 +193,16 @@
   </si>
   <si>
     <t>Camios a la libertad perimetral derecha Oe6</t>
+  </si>
+  <si>
+    <t>CUPOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,17 +211,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -274,13 +290,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -288,8 +305,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -309,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -605,239 +628,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B8AC53-B0CE-4F6C-8DB1-4409F3645CAF}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>